<commit_message>
Add municipal water providers layer, issue #2
</commit_message>
<xml_diff>
--- a/workflow/SupportingData/Municipal-WaterRentals/data/ditch-water-rentals.xlsx
+++ b/workflow/SupportingData/Municipal-WaterRentals/data/ditch-water-rentals.xlsx
@@ -57,15 +57,9 @@
     <t>no</t>
   </si>
   <si>
-    <t>DitchCompany</t>
-  </si>
-  <si>
     <t>https://www.newcache.com/rental-water</t>
   </si>
   <si>
-    <t>HasRentalProgramWebPage</t>
-  </si>
-  <si>
     <t>The New Cache La Poudre Irrigating Company</t>
   </si>
   <si>
@@ -73,6 +67,12 @@
   </si>
   <si>
     <t>North Poudre Irrigation Company</t>
+  </si>
+  <si>
+    <t>DitchCompanyName</t>
+  </si>
+  <si>
+    <t>HasWebPage</t>
   </si>
 </sst>
 </file>
@@ -462,27 +462,27 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="41.6640625" customWidth="1"/>
     <col min="2" max="2" width="43.109375" customWidth="1"/>
-    <col min="3" max="3" width="26.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -493,10 +493,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -510,10 +510,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>

</xml_diff>